<commit_message>
rewrote SFTP connection as a function for multiple calls. implemented plot variables for LeechT and LeechT. added LeechP mech picture.
</commit_message>
<xml_diff>
--- a/tmp/log_ESTIM.xlsx
+++ b/tmp/log_ESTIM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -98,6 +98,21 @@
   </si>
   <si>
     <t>14:47:22</t>
+  </si>
+  <si>
+    <t>2018.03.08</t>
+  </si>
+  <si>
+    <t>17:47:10</t>
+  </si>
+  <si>
+    <t>LeechT</t>
+  </si>
+  <si>
+    <t>17:47:36</t>
+  </si>
+  <si>
+    <t>17:47:43</t>
   </si>
 </sst>
 </file>
@@ -420,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -900,6 +915,120 @@
         <v>15</v>
       </c>
     </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="n">
+        <v>20</v>
+      </c>
+      <c r="E13" t="n">
+        <v>310</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3499</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J13" t="n">
+        <v>12</v>
+      </c>
+      <c r="K13" t="n">
+        <v>3.501129396579542</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.03874718679669917</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="n">
+        <v>20</v>
+      </c>
+      <c r="E14" t="n">
+        <v>310</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3499</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J14" t="n">
+        <v>12</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3.501129396579542</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.03874718679669917</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="n">
+        <v>20</v>
+      </c>
+      <c r="E15" t="n">
+        <v>300</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3499</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J15" t="n">
+        <v>12</v>
+      </c>
+      <c r="K15" t="n">
+        <v>3.501167055685228</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.0387467700258398</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
changed firing rate unit from kHz to Hz in info table
</commit_message>
<xml_diff>
--- a/tmp/log_ESTIM.xlsx
+++ b/tmp/log_ESTIM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -113,6 +113,36 @@
   </si>
   <si>
     <t>17:47:43</t>
+  </si>
+  <si>
+    <t>2018.03.09</t>
+  </si>
+  <si>
+    <t>15:32:32</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>15:52:41</t>
+  </si>
+  <si>
+    <t>2018.03.28</t>
+  </si>
+  <si>
+    <t>14:40:02</t>
+  </si>
+  <si>
+    <t>14:40:03</t>
+  </si>
+  <si>
+    <t>2018.03.29</t>
+  </si>
+  <si>
+    <t>16:48:14</t>
+  </si>
+  <si>
+    <t>16:48:15</t>
   </si>
 </sst>
 </file>
@@ -435,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -1029,6 +1059,310 @@
         <v>0.0387467700258398</v>
       </c>
     </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E16" t="n">
+        <v>50</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="H16" t="n">
+        <v>3495</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>37.67676767676767</v>
+      </c>
+      <c r="L16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" t="n">
+        <v>50</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="H17" t="n">
+        <v>3495</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>37.67676767676767</v>
+      </c>
+      <c r="L17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" t="n">
+        <v>50</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="H18" t="n">
+        <v>3495</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>32.62626262626263</v>
+      </c>
+      <c r="L18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E19" t="n">
+        <v>50</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="H19" t="n">
+        <v>3495</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>32.62626262626263</v>
+      </c>
+      <c r="L19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" t="n">
+        <v>50</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="H20" t="n">
+        <v>3495</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" t="n">
+        <v>32.62626262626263</v>
+      </c>
+      <c r="L20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="n">
+        <v>11</v>
+      </c>
+      <c r="E21" t="n">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>3499</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>27.85571142284569</v>
+      </c>
+      <c r="L21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="n">
+        <v>11</v>
+      </c>
+      <c r="E22" t="n">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>3499</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>27.85571142284569</v>
+      </c>
+      <c r="L22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="n">
+        <v>11</v>
+      </c>
+      <c r="E23" t="n">
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>3499</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" t="n">
+        <v>27.85571142284569</v>
+      </c>
+      <c r="L23" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>